<commit_message>
Added excluded dates to example input
</commit_message>
<xml_diff>
--- a/example_input.xlsx
+++ b/example_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t xml:space="preserve">Day(s) / Event(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holidays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.03.2018 – 27.03.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renovation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.06.2018| 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gym blocked</t>
   </si>
   <si>
     <t xml:space="preserve">Day</t>
@@ -208,8 +223,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -283,8 +298,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,7 +319,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,28 +351,31 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -373,46 +395,75 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>43101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>43281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>43210</v>
       </c>
     </row>
   </sheetData>
@@ -438,67 +489,70 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>14</v>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="n">
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="n">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -525,120 +579,123 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>43142</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>43170</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>43142</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0.791666666666667</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>43114</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>43170</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0.791666666666667</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>43204</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>43114</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>43204</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>25</v>
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -665,397 +722,399 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.43877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1001</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3" t="n">
+      <c r="J2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1002</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3" t="n">
+      <c r="J3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1003</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="n">
+      <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>1004</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3" t="n">
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>1005</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="0" t="n">
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3" t="n">
+      <c r="J6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>1006</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3" t="n">
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>1007</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3" t="n">
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>1008</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3" t="n">
+      <c r="J9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>1009</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3" t="n">
+      <c r="J10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>1010</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3" t="n">
+      <c r="J11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>1011</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="0" t="n">
+      <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="J12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3" t="n">
+      <c r="J12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>1012</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3" t="n">
+      <c r="J13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>1013</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3" t="n">
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>1014</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3" t="n">
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>1015</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="0" t="n">
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="J16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3" t="n">
+      <c r="J16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>1016</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="0" t="n">
+      <c r="B17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="3" t="n">
+      <c r="J17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>1017</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="0" t="n">
+      <c r="B18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="J18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3" t="n">
+      <c r="J18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>1018</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="0" t="n">
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="3" t="n">
+      <c r="J19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>1019</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="0" t="n">
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="J20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3" t="n">
+      <c r="J20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>1020</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3" t="n">
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="5" t="n">
         <v>43089</v>
       </c>
     </row>
@@ -1083,30 +1142,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="4" t="n">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>57</v>
+      <c r="C2" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Previously hard-coded settings can now be changed via the settings sheet.
</commit_message>
<xml_diff>
--- a/example_input.xlsx
+++ b/example_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -210,10 +210,49 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
-    <t xml:space="preserve">Cool down time in days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The worker will not be selected during the cool down time after his last action</t>
+    <t xml:space="preserve">Timezone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europe/Berlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time zone of the user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legendDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text for the legend of the output file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legendDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legendTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legendComment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cooldowntime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The worker will not be selected during the cool down time after his last action.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impactOfPreferredEvent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increasing this values makes it more likely that people are selected for preferred events.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shuffle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If several workers have the same ranking value, this settings decides whether they are selected randomly. If shuffle = false, the first worker is selected.</t>
   </si>
 </sst>
 </file>
@@ -297,7 +336,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,8 +357,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -346,6 +397,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -395,8 +449,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,7 +536,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,7 +628,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,8 +772,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,16 +1184,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="59.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,19 +1205,105 @@
       <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>62</v>
+      <c r="C10" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified example input to show how the reciprocal "works without" is used
</commit_message>
<xml_diff>
--- a/example_input.xlsx
+++ b/example_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -138,7 +138,7 @@
     <t xml:space="preserve">Works with (only one)</t>
   </si>
   <si>
-    <t xml:space="preserve">Works without (only one)</t>
+    <t xml:space="preserve">Works without</t>
   </si>
   <si>
     <t xml:space="preserve">Count of last period</t>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t xml:space="preserve">Oliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1002; 1009; 1004</t>
   </si>
   <si>
     <t xml:space="preserve">Jack</t>
@@ -259,10 +262,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -336,7 +340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,6 +377,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -398,7 +406,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,9 +457,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,9 +543,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,9 +633,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.62755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.2091836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,15 +772,20 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.61224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.33163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.43877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.2704081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.4591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,6 +836,9 @@
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="J2" s="1" t="n">
         <v>0</v>
       </c>
@@ -838,7 +851,7 @@
         <v>1002</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>102</v>
@@ -855,7 +868,7 @@
         <v>1003</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>101</v>
@@ -875,7 +888,7 @@
         <v>1004</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>102</v>
@@ -892,7 +905,7 @@
         <v>1005</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>102</v>
@@ -909,7 +922,7 @@
         <v>1006</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
@@ -926,7 +939,7 @@
         <v>1007</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
@@ -943,7 +956,7 @@
         <v>1008</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>101</v>
@@ -960,7 +973,7 @@
         <v>1009</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>102</v>
@@ -977,7 +990,7 @@
         <v>1010</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>101</v>
@@ -997,7 +1010,7 @@
         <v>1011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>102</v>
@@ -1017,7 +1030,7 @@
         <v>1012</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>102</v>
@@ -1034,7 +1047,7 @@
         <v>1013</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -1051,7 +1064,7 @@
         <v>1014</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
@@ -1068,7 +1081,7 @@
         <v>1015</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>101</v>
@@ -1088,7 +1101,7 @@
         <v>1016</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>102</v>
@@ -1105,7 +1118,7 @@
         <v>1017</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>101</v>
@@ -1122,7 +1135,7 @@
         <v>1018</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>102</v>
@@ -1139,7 +1152,7 @@
         <v>1019</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>102</v>
@@ -1156,7 +1169,7 @@
         <v>1020</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
@@ -1187,15 +1200,15 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>19</v>
@@ -1216,13 +1229,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,18 +1245,18 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>25</v>
@@ -1252,7 +1265,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>16</v>
@@ -1261,7 +1274,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -1275,35 +1288,35 @@
     </row>
     <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="B12" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="C12" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>